<commit_message>
Updated with correlation score
</commit_message>
<xml_diff>
--- a/Glioblastoma_markers.xlsx
+++ b/Glioblastoma_markers.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="22260" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="203">
   <si>
     <t>Upregulated</t>
   </si>
@@ -625,12 +625,15 @@
   </si>
   <si>
     <t>'LINC00342'</t>
+  </si>
+  <si>
+    <t>Correlation score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -934,828 +937,1437 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C101"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>202</v>
+      </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2">
+        <v>0.41035033787955399</v>
+      </c>
       <c r="C2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D2">
+        <v>0.28636774162591699</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3">
+        <v>0.387798696088338</v>
+      </c>
       <c r="C3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D3">
+        <v>0.27344846906105102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4">
+        <v>0.35076279087266599</v>
+      </c>
       <c r="C4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D4">
+        <v>0.26906834947296199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5">
+        <v>0.34588732798498201</v>
+      </c>
       <c r="C5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D5">
+        <v>0.25975295520595199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>6</v>
       </c>
+      <c r="B6">
+        <v>0.34178290621367702</v>
+      </c>
       <c r="C6" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6">
+        <v>0.25387475047647301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>7</v>
       </c>
+      <c r="B7">
+        <v>0.33951709955967302</v>
+      </c>
       <c r="C7" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7">
+        <v>0.25382590508733099</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>8</v>
       </c>
+      <c r="B8">
+        <v>0.336444122917678</v>
+      </c>
       <c r="C8" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D8">
+        <v>0.25117152691483802</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>9</v>
       </c>
+      <c r="B9">
+        <v>0.33554097136973898</v>
+      </c>
       <c r="C9" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D9">
+        <v>0.24649214493858601</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>10</v>
       </c>
+      <c r="B10">
+        <v>0.33279576571012998</v>
+      </c>
       <c r="C10" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D10">
+        <v>0.245046626148504</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>11</v>
       </c>
+      <c r="B11">
+        <v>0.32866200327359901</v>
+      </c>
       <c r="C11" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D11">
+        <v>0.24427154378854701</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>12</v>
       </c>
+      <c r="B12">
+        <v>0.32753438804969298</v>
+      </c>
       <c r="C12" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D12">
+        <v>0.24337764112155599</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>13</v>
       </c>
+      <c r="B13">
+        <v>0.31563634234138199</v>
+      </c>
       <c r="C13" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D13">
+        <v>0.24322965607265601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>14</v>
       </c>
+      <c r="B14">
+        <v>0.314628435373145</v>
+      </c>
       <c r="C14" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D14">
+        <v>0.242508649166118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>15</v>
       </c>
+      <c r="B15">
+        <v>0.30275280483176498</v>
+      </c>
       <c r="C15" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D15">
+        <v>0.23827299864267501</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>16</v>
       </c>
+      <c r="B16">
+        <v>0.30036604384374199</v>
+      </c>
       <c r="C16" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D16">
+        <v>0.23130021756702401</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>17</v>
       </c>
+      <c r="B17">
+        <v>0.29917950055929299</v>
+      </c>
       <c r="C17" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D17">
+        <v>0.23123654780779501</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>18</v>
       </c>
+      <c r="B18">
+        <v>0.29506232752965</v>
+      </c>
       <c r="C18" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D18">
+        <v>0.23094068829783501</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>19</v>
       </c>
+      <c r="B19">
+        <v>0.29425827246498099</v>
+      </c>
       <c r="C19" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D19">
+        <v>0.23008139026338101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>20</v>
       </c>
+      <c r="B20">
+        <v>0.29315029835946399</v>
+      </c>
       <c r="C20" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D20">
+        <v>0.22990863999606401</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>21</v>
       </c>
+      <c r="B21">
+        <v>0.28652759548506102</v>
+      </c>
       <c r="C21" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D21">
+        <v>0.225681688797369</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>22</v>
       </c>
+      <c r="B22">
+        <v>0.286337820427152</v>
+      </c>
       <c r="C22" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D22">
+        <v>0.22551907428342999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>23</v>
       </c>
+      <c r="B23">
+        <v>0.28559525667666702</v>
+      </c>
       <c r="C23" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D23">
+        <v>0.22537981612562</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>24</v>
       </c>
+      <c r="B24">
+        <v>0.28398225314118197</v>
+      </c>
       <c r="C24" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D24">
+        <v>0.22470190092673201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>25</v>
       </c>
+      <c r="B25">
+        <v>0.28296300044634398</v>
+      </c>
       <c r="C25" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D25">
+        <v>0.221654634507436</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>26</v>
       </c>
+      <c r="B26">
+        <v>0.28131818017558402</v>
+      </c>
       <c r="C26" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D26">
+        <v>0.22151148734187701</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>27</v>
       </c>
+      <c r="B27">
+        <v>0.27995850723480997</v>
+      </c>
       <c r="C27" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D27">
+        <v>0.21992930825770499</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>28</v>
       </c>
+      <c r="B28">
+        <v>0.27946410365250901</v>
+      </c>
       <c r="C28" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D28">
+        <v>0.21952159601391799</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>29</v>
       </c>
+      <c r="B29">
+        <v>0.279372857090187</v>
+      </c>
       <c r="C29" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D29">
+        <v>0.21920581781245399</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>30</v>
       </c>
+      <c r="B30">
+        <v>0.27930105600321298</v>
+      </c>
       <c r="C30" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D30">
+        <v>0.21692521858928601</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>31</v>
       </c>
+      <c r="B31">
+        <v>0.27825308012385802</v>
+      </c>
       <c r="C31" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D31">
+        <v>0.21640130241322</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>32</v>
       </c>
+      <c r="B32">
+        <v>0.27436668637009898</v>
+      </c>
       <c r="C32" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D32">
+        <v>0.21549006502746501</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>33</v>
       </c>
+      <c r="B33">
+        <v>0.27268366394350801</v>
+      </c>
       <c r="C33" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D33">
+        <v>0.21491163030853599</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>34</v>
       </c>
+      <c r="B34">
+        <v>0.27231654116639298</v>
+      </c>
       <c r="C34" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D34">
+        <v>0.214493976919267</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>35</v>
       </c>
+      <c r="B35">
+        <v>0.27148040436528398</v>
+      </c>
       <c r="C35" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D35">
+        <v>0.21401599791348999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>36</v>
       </c>
+      <c r="B36">
+        <v>0.27082547391759398</v>
+      </c>
       <c r="C36" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D36">
+        <v>0.21222192952682001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>37</v>
       </c>
+      <c r="B37">
+        <v>0.27066436763016799</v>
+      </c>
       <c r="C37" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D37">
+        <v>0.21139366538006199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>38</v>
       </c>
+      <c r="B38">
+        <v>0.26972511627201101</v>
+      </c>
       <c r="C38" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D38">
+        <v>0.210065802436632</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>39</v>
       </c>
+      <c r="B39">
+        <v>0.26926168849883397</v>
+      </c>
       <c r="C39" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D39">
+        <v>0.20856777625815701</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>40</v>
       </c>
+      <c r="B40">
+        <v>0.26908608324695099</v>
+      </c>
       <c r="C40" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D40">
+        <v>0.20819881490007699</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>41</v>
       </c>
+      <c r="B41">
+        <v>0.268792490154381</v>
+      </c>
       <c r="C41" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D41">
+        <v>0.207947299139779</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>42</v>
       </c>
+      <c r="B42">
+        <v>0.26701311387333199</v>
+      </c>
       <c r="C42" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D42">
+        <v>0.207890065701473</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>43</v>
       </c>
+      <c r="B43">
+        <v>0.26695395683598999</v>
+      </c>
       <c r="C43" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D43">
+        <v>0.20746765502341999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>44</v>
       </c>
+      <c r="B44">
+        <v>0.26365403780551999</v>
+      </c>
       <c r="C44" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D44">
+        <v>0.20690607215319501</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>45</v>
       </c>
+      <c r="B45">
+        <v>0.26365187379299498</v>
+      </c>
       <c r="C45" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D45">
+        <v>0.20686838015651099</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>46</v>
       </c>
+      <c r="B46">
+        <v>0.26317572664516398</v>
+      </c>
       <c r="C46" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D46">
+        <v>0.20671252253785</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>47</v>
       </c>
+      <c r="B47">
+        <v>0.262998014265798</v>
+      </c>
       <c r="C47" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D47">
+        <v>0.20591814476117201</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>48</v>
       </c>
+      <c r="B48">
+        <v>0.26276293765969899</v>
+      </c>
       <c r="C48" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D48">
+        <v>0.20589393578017301</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>49</v>
       </c>
+      <c r="B49">
+        <v>0.259723736522881</v>
+      </c>
       <c r="C49" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D49">
+        <v>0.20394652787458201</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>50</v>
       </c>
+      <c r="B50">
+        <v>0.25936857745931802</v>
+      </c>
       <c r="C50" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D50">
+        <v>0.203067941988368</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>51</v>
       </c>
+      <c r="B51">
+        <v>0.25895758186708701</v>
+      </c>
       <c r="C51" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D51">
+        <v>0.20281676876081001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>52</v>
       </c>
+      <c r="B52">
+        <v>0.25865393751246801</v>
+      </c>
       <c r="C52" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D52">
+        <v>0.201109817842582</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>53</v>
       </c>
+      <c r="B53">
+        <v>0.258231035992461</v>
+      </c>
       <c r="C53" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D53">
+        <v>0.201014218530505</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>54</v>
       </c>
+      <c r="B54">
+        <v>0.25797217076392498</v>
+      </c>
       <c r="C54" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D54">
+        <v>0.20100878064456801</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>55</v>
       </c>
+      <c r="B55">
+        <v>0.25597124838126001</v>
+      </c>
       <c r="C55" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D55">
+        <v>0.20068390587418</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>56</v>
       </c>
+      <c r="B56">
+        <v>0.25566409529283701</v>
+      </c>
       <c r="C56" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D56">
+        <v>0.20036914733008299</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>57</v>
       </c>
+      <c r="B57">
+        <v>0.25553690914000399</v>
+      </c>
       <c r="C57" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D57">
+        <v>0.19948125041741799</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>58</v>
       </c>
+      <c r="B58">
+        <v>0.25493553632820398</v>
+      </c>
       <c r="C58" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D58">
+        <v>0.19859044766603601</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>59</v>
       </c>
+      <c r="B59">
+        <v>0.25446290903009799</v>
+      </c>
       <c r="C59" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D59">
+        <v>0.197920481210062</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>60</v>
       </c>
+      <c r="B60">
+        <v>0.25318715262465202</v>
+      </c>
       <c r="C60" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D60">
+        <v>0.196348776981531</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>61</v>
       </c>
+      <c r="B61">
+        <v>0.25281672688384199</v>
+      </c>
       <c r="C61" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D61">
+        <v>0.195908518640691</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>62</v>
       </c>
+      <c r="B62">
+        <v>0.251815343651487</v>
+      </c>
       <c r="C62" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D62">
+        <v>0.19574393905774701</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>63</v>
       </c>
+      <c r="B63">
+        <v>0.25103750002649899</v>
+      </c>
       <c r="C63" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D63">
+        <v>0.19520865481538299</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>64</v>
       </c>
+      <c r="B64">
+        <v>0.25102637322030003</v>
+      </c>
       <c r="C64" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D64">
+        <v>0.19467641936996899</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>65</v>
       </c>
+      <c r="B65">
+        <v>0.24959840543335099</v>
+      </c>
       <c r="C65" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D65">
+        <v>0.19396149205780699</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>66</v>
       </c>
+      <c r="B66">
+        <v>0.24957585985054301</v>
+      </c>
       <c r="C66" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D66">
+        <v>0.19372107644252701</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>67</v>
       </c>
+      <c r="B67">
+        <v>0.24799225752281701</v>
+      </c>
       <c r="C67" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D67">
+        <v>0.19364585692066599</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>68</v>
       </c>
+      <c r="B68">
+        <v>0.247245824583884</v>
+      </c>
       <c r="C68" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D68">
+        <v>0.19332384172720901</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>69</v>
       </c>
+      <c r="B69">
+        <v>0.24687831872108701</v>
+      </c>
       <c r="C69" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D69">
+        <v>0.192691184724023</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>70</v>
       </c>
+      <c r="B70">
+        <v>0.24589358075623</v>
+      </c>
       <c r="C70" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D70">
+        <v>0.19130665411217099</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>71</v>
       </c>
+      <c r="B71">
+        <v>0.24552100496269499</v>
+      </c>
       <c r="C71" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D71">
+        <v>0.19022514212806299</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>72</v>
       </c>
+      <c r="B72">
+        <v>0.24518565032991499</v>
+      </c>
       <c r="C72" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D72">
+        <v>0.18988112791494999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>73</v>
       </c>
+      <c r="B73">
+        <v>0.24458497131262</v>
+      </c>
       <c r="C73" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D73">
+        <v>0.189526583755143</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>74</v>
       </c>
+      <c r="B74">
+        <v>0.244448409891762</v>
+      </c>
       <c r="C74" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D74">
+        <v>0.18923514042600101</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>75</v>
       </c>
+      <c r="B75">
+        <v>0.24415110326841299</v>
+      </c>
       <c r="C75" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D75">
+        <v>0.18753626496387801</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>76</v>
       </c>
+      <c r="B76">
+        <v>0.24353134383545599</v>
+      </c>
       <c r="C76" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D76">
+        <v>0.18748007270412601</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
         <v>77</v>
       </c>
+      <c r="B77">
+        <v>0.24297926631140701</v>
+      </c>
       <c r="C77" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D77">
+        <v>0.186640587840911</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>78</v>
       </c>
+      <c r="B78">
+        <v>0.24196718911427101</v>
+      </c>
       <c r="C78" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D78">
+        <v>0.185458451091121</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>79</v>
       </c>
+      <c r="B79">
+        <v>0.24180663385828899</v>
+      </c>
       <c r="C79" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D79">
+        <v>0.18521905609625899</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
         <v>80</v>
       </c>
+      <c r="B80">
+        <v>0.24146859934136999</v>
+      </c>
       <c r="C80" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D80">
+        <v>0.18519520966886899</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>81</v>
       </c>
+      <c r="B81">
+        <v>0.24104484328728901</v>
+      </c>
       <c r="C81" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D81">
+        <v>0.183345965238323</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>82</v>
       </c>
+      <c r="B82">
+        <v>0.24012561861807499</v>
+      </c>
       <c r="C82" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D82">
+        <v>0.182376365332584</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>83</v>
       </c>
+      <c r="B83">
+        <v>0.23998876451686599</v>
+      </c>
       <c r="C83" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D83">
+        <v>0.182323400482794</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
         <v>84</v>
       </c>
+      <c r="B84">
+        <v>0.23989360819859701</v>
+      </c>
       <c r="C84" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D84">
+        <v>0.18211977146467501</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
         <v>85</v>
       </c>
+      <c r="B85">
+        <v>0.23945089212218101</v>
+      </c>
       <c r="C85" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D85">
+        <v>0.18198568863386699</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
         <v>86</v>
       </c>
+      <c r="B86">
+        <v>0.239041622034837</v>
+      </c>
       <c r="C86" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D86">
+        <v>0.18187409384440301</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
         <v>87</v>
       </c>
+      <c r="B87">
+        <v>0.238478233295388</v>
+      </c>
       <c r="C87" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D87">
+        <v>0.18114341067136699</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
         <v>88</v>
       </c>
+      <c r="B88">
+        <v>0.238198550132035</v>
+      </c>
       <c r="C88" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D88">
+        <v>0.180868437541924</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
         <v>89</v>
       </c>
+      <c r="B89">
+        <v>0.23800181735461401</v>
+      </c>
       <c r="C89" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D89">
+        <v>0.180142165507409</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>90</v>
       </c>
+      <c r="B90">
+        <v>0.23752967859212101</v>
+      </c>
       <c r="C90" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D90">
+        <v>0.17963664659071499</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
         <v>91</v>
       </c>
+      <c r="B91">
+        <v>0.237387562097234</v>
+      </c>
       <c r="C91" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D91">
+        <v>0.17952991553831901</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
         <v>92</v>
       </c>
+      <c r="B92">
+        <v>0.237079658549814</v>
+      </c>
       <c r="C92" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D92">
+        <v>0.17831159950804601</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>93</v>
       </c>
+      <c r="B93">
+        <v>0.236978746638664</v>
+      </c>
       <c r="C93" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D93">
+        <v>0.17820441961957301</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>94</v>
       </c>
+      <c r="B94">
+        <v>0.23689401865419399</v>
+      </c>
       <c r="C94" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D94">
+        <v>0.178005597952682</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>95</v>
       </c>
+      <c r="B95">
+        <v>0.23597676125106601</v>
+      </c>
       <c r="C95" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D95">
+        <v>0.17750706243935599</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
         <v>96</v>
       </c>
+      <c r="B96">
+        <v>0.23523594488192001</v>
+      </c>
       <c r="C96" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D96">
+        <v>0.177412413252309</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
         <v>97</v>
       </c>
+      <c r="B97">
+        <v>0.23445640432186499</v>
+      </c>
       <c r="C97" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D97">
+        <v>0.177378639981598</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
         <v>98</v>
       </c>
+      <c r="B98">
+        <v>0.234255141554608</v>
+      </c>
       <c r="C98" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D98">
+        <v>0.176753330706129</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
         <v>99</v>
       </c>
+      <c r="B99">
+        <v>0.23400858456653401</v>
+      </c>
       <c r="C99" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D99">
+        <v>0.17624023098255501</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
         <v>100</v>
       </c>
+      <c r="B100">
+        <v>0.23388403398566601</v>
+      </c>
       <c r="C100" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D100">
+        <v>0.176119156246619</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
         <v>101</v>
       </c>
+      <c r="B101">
+        <v>0.23378939539426499</v>
+      </c>
       <c r="C101" t="s">
         <v>201</v>
+      </c>
+      <c r="D101">
+        <v>0.17507087471223601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>